<commit_message>
Can load to N4j: - Country - Region - CropGroup - CropClass - CropSubClass - CropVariety - CropDescription
and relations between them
</commit_message>
<xml_diff>
--- a/loader/src/main/resources/CropDescription.xlsx
+++ b/loader/src/main/resources/CropDescription.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23525"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAB2095E-5B72-4A40-82E2-26B0FA13B86F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5B377A8-B4AF-44EC-8C44-7BDD134FB2CC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,25 +106,25 @@
     <t>5364988c-75f5-4d0c-ace9-145b2d859f01</t>
   </si>
   <si>
-    <t>Durum Protein 13%</t>
+    <t>Durum Protein 13</t>
   </si>
   <si>
     <t>8a33e8a5-dbb2-426a-8d9b-64ecd07e4d6f</t>
   </si>
   <si>
-    <t>Durum Protein 14%</t>
+    <t>Durum Protein 14</t>
   </si>
   <si>
     <t>a105e759-38cc-4d71-8927-417df401f745</t>
   </si>
   <si>
-    <t>Durum Protein 15%</t>
+    <t>Durum Protein 15</t>
   </si>
   <si>
     <t>d0529c06-5152-4195-b67a-a7733a8d1d8b</t>
   </si>
   <si>
-    <t>Durum Protein 16%</t>
+    <t>Durum Protein 16</t>
   </si>
   <si>
     <t>d47e411e-632a-41d8-8c91-a9ec9b5b054e</t>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:G442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Corrected Test UseCases.cypher, UseCasesWithRelations.cypher, UseCasesExpectedAnswers.json and RelationsReferenceIdTest.java as per latest ontology version (ODX_Crop_V3)
</commit_message>
<xml_diff>
--- a/loader/src/main/resources/CropDescription.xlsx
+++ b/loader/src/main/resources/CropDescription.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23720"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5B377A8-B4AF-44EC-8C44-7BDD134FB2CC}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3BCA35A7-9211-4143-8AB1-E4050CC4582C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,25 +106,25 @@
     <t>5364988c-75f5-4d0c-ace9-145b2d859f01</t>
   </si>
   <si>
-    <t>Durum Protein 13</t>
+    <t>Durum Protein 13%</t>
   </si>
   <si>
     <t>8a33e8a5-dbb2-426a-8d9b-64ecd07e4d6f</t>
   </si>
   <si>
-    <t>Durum Protein 14</t>
+    <t>Durum Protein 14%</t>
   </si>
   <si>
     <t>a105e759-38cc-4d71-8927-417df401f745</t>
   </si>
   <si>
-    <t>Durum Protein 15</t>
+    <t>Durum Protein 15%</t>
   </si>
   <si>
     <t>d0529c06-5152-4195-b67a-a7733a8d1d8b</t>
   </si>
   <si>
-    <t>Durum Protein 16</t>
+    <t>Durum Protein 16%</t>
   </si>
   <si>
     <t>d47e411e-632a-41d8-8c91-a9ec9b5b054e</t>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:G442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2:G442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>